<commit_message>
Semana 10: Tercer grado
</commit_message>
<xml_diff>
--- a/santillana-recursos/semana_10/LGS2_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
+++ b/santillana-recursos/semana_10/LGS2_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fceron/Desktop/APRENDE EN CASA/SEMANA 10/DEFINITIVOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos.ciddelapaz/Library/Mobile Documents/com~apple~CloudDocs/Dev/GitHub/gavi/santillana-recursos/semana_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8020CB3C-4F8F-B343-AC87-92374EE67A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72388536-8F45-674E-ADD5-665E51373E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="460" windowWidth="33160" windowHeight="22880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LGS2 - Semana 10" sheetId="1" r:id="rId1"/>
@@ -793,7 +793,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -819,9 +819,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -831,9 +828,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -885,9 +879,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -953,9 +944,6 @@
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1318,10 +1306,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1329,7 +1317,7 @@
     <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
@@ -1343,28 +1331,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="74"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1385,610 +1373,574 @@
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="62" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="67"/>
+      <c r="H4" s="63"/>
     </row>
     <row r="5" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="20" t="s">
         <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="61" t="s">
+      <c r="G5" s="54"/>
+      <c r="H5" s="57" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="78"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="51" t="s">
+      <c r="G6" s="34"/>
+      <c r="H6" s="48" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="78"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="51" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="48" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="78"/>
-      <c r="B8" s="46" t="s">
+      <c r="A8" s="74"/>
+      <c r="B8" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="51" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-    </row>
-    <row r="10" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
+    <row r="9" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B9" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F9" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-    </row>
-    <row r="11" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
-      <c r="B11" s="10" t="s">
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
+    </row>
+    <row r="10" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F10" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="51" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="48" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
-      <c r="B12" s="10" t="s">
+    <row r="11" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="65"/>
+      <c r="B11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F11" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="51" t="s">
+      <c r="G11" s="53"/>
+      <c r="H11" s="48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="10" t="s">
+    <row r="12" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="65"/>
+      <c r="B12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>98</v>
       </c>
+      <c r="E12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="54"/>
+      <c r="H12" s="48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="67"/>
+      <c r="B13" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
-      <c r="B14" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="53"/>
+      <c r="H13" s="48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="65"/>
+      <c r="B15" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="49"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="65"/>
+      <c r="B16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="50"/>
+      <c r="H16" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="65"/>
+      <c r="B17" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="56"/>
+      <c r="H17" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="75"/>
+      <c r="B18" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="51" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-    </row>
-    <row r="16" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="42" t="s">
+      <c r="D18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="69"/>
-      <c r="B17" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="42" t="s">
+      <c r="D19" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="65"/>
+      <c r="B20" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D20" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="58"/>
+    </row>
+    <row r="21" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="66"/>
+      <c r="B21" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="66"/>
+      <c r="B22" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="67"/>
+      <c r="B23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" s="48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="53"/>
+    </row>
+    <row r="25" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="65"/>
+      <c r="B25" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="66"/>
+      <c r="B26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="66"/>
+      <c r="B27" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E27" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F27" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="36"/>
-    </row>
-    <row r="18" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="69"/>
-      <c r="B18" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="53"/>
-      <c r="H18" s="51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="69"/>
-      <c r="B19" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="60"/>
-      <c r="H19" s="51" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="79"/>
-      <c r="B20" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="42" t="s">
+      <c r="G27" s="60"/>
+      <c r="H27" s="57"/>
+    </row>
+    <row r="28" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="67"/>
+      <c r="B28" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-    </row>
-    <row r="22" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-    </row>
-    <row r="23" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="69"/>
-      <c r="B23" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="62"/>
-    </row>
-    <row r="24" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="70"/>
-      <c r="B24" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="70"/>
-      <c r="B25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="53"/>
-      <c r="H25" s="51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
-      <c r="B26" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="63"/>
-      <c r="H26" s="51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-    </row>
-    <row r="28" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" s="57"/>
-    </row>
-    <row r="29" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="69"/>
-      <c r="B29" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="H29" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="70"/>
-      <c r="B30" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="53"/>
-      <c r="H30" s="51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="70"/>
-      <c r="B31" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="64"/>
-      <c r="H31" s="61"/>
-    </row>
-    <row r="32" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="71"/>
-      <c r="B32" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="50" t="s">
+      <c r="D28" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E28" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="48" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="43"/>
+      <c r="H28" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A18"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>